<commit_message>
add more chart test cases have no headers add scatter chart test case which has no series name column
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/book/insert-charts.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/book/insert-charts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>date</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>3D bar</t>
+  </si>
+  <si>
+    <t>Daily Ranfall</t>
+  </si>
+  <si>
+    <t>Particulate</t>
   </si>
 </sst>
 </file>
@@ -518,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:N240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -772,8 +778,85 @@
     <row r="24" spans="1:12">
       <c r="A24" s="2"/>
     </row>
-    <row r="39" spans="1:12" ht="18.75">
-      <c r="A39" s="3"/>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B31">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>4.3</v>
+      </c>
+      <c r="B32">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>5.7</v>
+      </c>
+      <c r="B33">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>5.4</v>
+      </c>
+      <c r="B34">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>5.9</v>
+      </c>
+      <c r="B35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37">
+        <v>3.6</v>
+      </c>
+      <c r="B37">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38">
+        <v>1.9</v>
+      </c>
+      <c r="B38">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39">
+        <v>7.3</v>
+      </c>
+      <c r="B39">
+        <v>104</v>
+      </c>
     </row>
     <row r="40" spans="1:12">
       <c r="L40" t="s">

</xml_diff>